<commit_message>
updated for recording utility
</commit_message>
<xml_diff>
--- a/bin/com/uat/xls/Users.xlsx
+++ b/bin/com/uat/xls/Users.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="59">
   <si>
     <t>Username</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>test1@gmail.com</t>
+  </si>
+  <si>
+    <t>test@click2cloud.com</t>
   </si>
 </sst>
 </file>
@@ -646,17 +649,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.140625" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -690,6 +693,17 @@
       </c>
       <c r="C3" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -706,7 +720,7 @@
           <x14:formula1>
             <xm:f>Sheet3!$C$4:$C$10</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C3</xm:sqref>
+          <xm:sqref>C2:C4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>